<commit_message>
Subo fotos del amplificador y voy actualizando las mediciones de ayer.
</commit_message>
<xml_diff>
--- a/Mediciones/Punto de reposo/Mediciones del TP.xlsx
+++ b/Mediciones/Punto de reposo/Mediciones del TP.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Polarización</t>
   </si>
@@ -140,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -164,17 +164,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thick">
@@ -195,51 +184,73 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -247,37 +258,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,8 +505,8 @@
   </sheetPr>
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G22" sqref="A1:G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -516,428 +522,524 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="11">
         <v>33.9</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="11">
         <v>5.4876499999999999E-4</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="11">
         <f>B3*C3</f>
         <v>1.8603133500000001E-2</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
+      <c r="E3" s="11">
+        <v>33.42</v>
+      </c>
+      <c r="F3" s="11">
+        <v>5.2857000000000002E-4</v>
+      </c>
+      <c r="G3" s="8">
+        <f>E3*F3</f>
+        <v>1.7664809400000002E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="11">
         <v>1.3140000000000001</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="11">
         <v>5.4876499999999999E-4</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="11">
         <f t="shared" ref="D4:D21" si="0">B4*C4</f>
         <v>7.2107721000000001E-4</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
+      <c r="E4" s="11">
+        <v>1.27</v>
+      </c>
+      <c r="F4" s="11">
+        <v>5.2817999999999995E-4</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" ref="G4:G21" si="1">E4*F4</f>
+        <v>6.7078859999999995E-4</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="B5" s="11">
         <v>31.8</v>
       </c>
-      <c r="D5" s="7">
-        <f t="shared" si="0"/>
-        <v>3.4980000000000004E-2</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
+      <c r="C5" s="11">
+        <v>1.0989999999999999E-3</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" si="0"/>
+        <v>3.4948199999999999E-2</v>
+      </c>
+      <c r="E5" s="11">
+        <v>31.62</v>
+      </c>
+      <c r="F5" s="11">
+        <v>1.07E-3</v>
+      </c>
+      <c r="G5" s="8">
+        <f t="shared" si="1"/>
+        <v>3.38334E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="11">
         <v>0.61055800000000005</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="11">
         <v>5.4876499999999999E-4</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="11">
         <f t="shared" si="0"/>
         <v>3.3505286087000003E-4</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
+      <c r="E6" s="11">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="F6" s="11">
+        <v>5.3227000000000005E-4</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" si="1"/>
+        <v>3.2574924000000003E-4</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="11">
         <v>34.576999999999998</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="11">
         <v>5.4876499999999999E-4</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="11">
         <f t="shared" si="0"/>
         <v>1.8974647405E-2</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
+      <c r="E7" s="11">
+        <v>34.32</v>
+      </c>
+      <c r="F7" s="11">
+        <v>5.375E-4</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" si="1"/>
+        <v>1.8447000000000002E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="11">
         <v>28.945</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="11">
         <v>9.7120000000000001E-3</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="11">
         <f t="shared" si="0"/>
         <v>0.28111384</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
+      <c r="E8" s="11">
+        <v>28.94</v>
+      </c>
+      <c r="F8" s="11">
+        <v>9.7300000000000008E-3</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="1"/>
+        <v>0.28158620000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="11">
         <v>30.234000000000002</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="11">
         <v>1.6922199999999999E-4</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="11">
         <f t="shared" si="0"/>
         <v>5.1162579479999996E-3</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
+      <c r="E9" s="11">
+        <v>28.27</v>
+      </c>
+      <c r="F9" s="11">
+        <v>1.4571000000000001E-4</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="1"/>
+        <v>4.1192217E-3</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="11">
         <v>30.902999999999999</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="11">
         <v>9.5490000000000002E-3</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="11">
         <f t="shared" si="0"/>
         <v>0.29509274699999999</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
+      <c r="E10" s="11">
+        <v>29.89</v>
+      </c>
+      <c r="F10" s="11">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="1"/>
+        <v>0.28694399999999998</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="11">
         <v>2.63</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="11">
         <v>9.476E-3</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="11">
         <f t="shared" si="0"/>
         <v>2.492188E-2</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="11">
         <v>14.147</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="11">
         <v>7.0229999999999997E-3</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="11">
         <f t="shared" si="0"/>
         <v>9.9354380999999992E-2</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="11">
         <v>20.233000000000001</v>
       </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="D13" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
+      <c r="C13" s="11">
+        <v>0</v>
+      </c>
+      <c r="D13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="11">
         <v>20.233000000000001</v>
       </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="D14" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
+      <c r="C14" s="11">
+        <v>0</v>
+      </c>
+      <c r="D14" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="11">
         <v>14.129</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="11">
         <v>7.8399999999999997E-3</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="11">
         <f t="shared" si="0"/>
         <v>0.11077136</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="7"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="11">
         <v>20.233000000000001</v>
       </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-      <c r="D16" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
+      <c r="C16" s="11">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="11">
         <v>14.757999999999999</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="11">
         <v>9.2329999999999995E-2</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="11">
         <f t="shared" si="0"/>
         <v>1.3626061399999998</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="11">
         <v>14.757</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="11">
         <v>9.3203999999999995E-2</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="11">
         <f t="shared" si="0"/>
         <v>1.3754114279999998</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="11">
         <v>20.233000000000001</v>
       </c>
-      <c r="C19" s="6">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
+      <c r="C19" s="11">
+        <v>0</v>
+      </c>
+      <c r="D19" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="11">
         <v>1.3220000000000001</v>
       </c>
-      <c r="C20" s="6">
-        <v>0</v>
-      </c>
-      <c r="D20" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
+      <c r="C20" s="11">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="14">
         <v>1.3080000000000001</v>
       </c>
-      <c r="C21" s="11">
-        <v>0</v>
-      </c>
-      <c r="D21" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9"/>
+      <c r="C21" s="14">
+        <v>0</v>
+      </c>
+      <c r="D21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="6">
         <f>SUM(D3:D21)</f>
-        <v>3.6280019449238692</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.6279701449238697</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="6">
+        <f>SUM(G3:G21)</f>
+        <v>0.64359116894000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B29" s="3"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>

</xml_diff>